<commit_message>
update register name to holding register
</commit_message>
<xml_diff>
--- a/documentation/Tabla_de_registros_HMI.xlsx
+++ b/documentation/Tabla_de_registros_HMI.xlsx
@@ -39,7 +39,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t xml:space="preserve">params</t>
+          <t xml:space="preserve">Params, start from 40006</t>
         </r>
       </text>
     </comment>
@@ -1715,7 +1715,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.57"/>
@@ -1740,7 +1740,7 @@
   </sheetPr>
   <dimension ref="A1:J294"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B70" colorId="64" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -1754,7 +1754,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="31.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="24.15"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.42"/>
   </cols>

</xml_diff>